<commit_message>
Updated Ep and Ip and EI average
</commit_message>
<xml_diff>
--- a/finished/Ar35/temp/36Ca.xlsx
+++ b/finished/Ar35/temp/36Ca.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\Files\A35\finished\Ar35\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74FAC5E-B914-459C-B3E3-95F2B67B813D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF7E3DD-618C-4EDA-BFBC-9926686824AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{80E8E01B-A04B-4992-8B74-8F4DE158A446}"/>
+    <workbookView xWindow="1416" yWindow="-36" windowWidth="12600" windowHeight="12000" activeTab="1" xr2:uid="{80E8E01B-A04B-4992-8B74-8F4DE158A446}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
   <si>
     <t>Ip</t>
   </si>
@@ -69,6 +69,18 @@
   <si>
     <t>1995Ga16</t>
   </si>
+  <si>
+    <t>inputs</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Ep</t>
+  </si>
 </sst>
 </file>
 
@@ -77,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,36 +98,43 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="9"/>
       <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="9"/>
       <color rgb="FF993300"/>
-      <name val="Cambria"/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="9"/>
       <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="9"/>
       <color rgb="FFFF0000"/>
-      <name val="Cambria"/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="9"/>
       <color rgb="FFFF0000"/>
-      <name val="Cambria"/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -171,6 +190,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -509,13 +534,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FCEC0C-CCF2-405C-89E2-FB3C4ADFF355}">
-  <dimension ref="A1:AG34"/>
+  <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="AD13" sqref="AD13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.21875" style="1" bestFit="1" customWidth="1"/>
@@ -543,13 +568,13 @@
     <col min="24" max="24" width="3.77734375" style="1" customWidth="1"/>
     <col min="25" max="25" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="34" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -572,6 +597,12 @@
       <c r="U1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="AA1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -613,16 +644,19 @@
       <c r="Y2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AA2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="12" x14ac:dyDescent="0.3">
       <c r="I3" s="3">
         <f>I14/36*35</f>
         <v>1397.0833333333333</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="5">
-        <f>K17*0.03/1.03+0.1</f>
-        <v>0.14951456310679612</v>
+        <f>K14</f>
+        <v>1.2</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="3">
@@ -630,8 +664,6 @@
         <v>1400</v>
       </c>
       <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
       <c r="Y3" s="6"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
@@ -644,12 +676,12 @@
         <v>39.094940233383809</v>
       </c>
       <c r="K4" s="5">
-        <f>K16</f>
-        <v>37.76407766990291</v>
+        <f t="shared" ref="K4:L11" si="2">K15</f>
+        <v>11.3</v>
       </c>
       <c r="L4" s="1">
-        <f>L16</f>
-        <v>10</v>
+        <f>L15</f>
+        <v>6</v>
       </c>
       <c r="M4" s="3">
         <f t="shared" si="0"/>
@@ -660,19 +692,19 @@
         <v>20.964862579157607</v>
       </c>
       <c r="O4" s="1">
-        <f>O16</f>
-        <v>37</v>
+        <f t="shared" ref="O4:P4" si="3">O15</f>
+        <v>9.3000000000000007</v>
       </c>
       <c r="P4" s="1">
-        <f>P16</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="Q4" s="3">
-        <f t="shared" ref="Q4:R5" si="2">Q15/36*35</f>
+        <f t="shared" ref="Q4:R5" si="4">Q15/36*35</f>
         <v>1659.5833333333333</v>
       </c>
       <c r="R4" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>17.5</v>
       </c>
       <c r="S4" s="1">
@@ -682,11 +714,11 @@
         <v>8</v>
       </c>
       <c r="U4" s="3">
-        <f t="shared" ref="U4:V4" si="3">U15/36*35</f>
+        <f t="shared" ref="U4:V4" si="5">U15/36*35</f>
         <v>1623.6111111111111</v>
       </c>
       <c r="V4" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>22.361111111111111</v>
       </c>
       <c r="W4" s="1">
@@ -701,24 +733,11 @@
       <c r="Z4" s="2">
         <v>0.8</v>
       </c>
-      <c r="AD4" s="3" t="str">
-        <f>TEXT(I4, "0")&amp;"("&amp;TEXT(J4, "0")&amp;") ("&amp;$I$1&amp;"), "</f>
-        <v xml:space="preserve">1676(39) (1997Tr05), </v>
-      </c>
-      <c r="AE4" s="3" t="str">
-        <f>TEXT(M4, "0")&amp;"("&amp;TEXT(N4, "0")&amp;") ("&amp;$M$1&amp;"), "</f>
-        <v xml:space="preserve">1645(21) (2001Lo11), </v>
-      </c>
-      <c r="AF4" s="3" t="str">
-        <f>TEXT(Q4, "0")&amp;"("&amp;TEXT(R4, "0")&amp;") ("&amp;$Q$1&amp;"), "</f>
-        <v xml:space="preserve">1660(18) (2007Do17), </v>
-      </c>
-      <c r="AG4" s="3" t="str">
-        <f>TEXT(U4, "0")&amp;"("&amp;TEXT(V4, "0")&amp;") ("&amp;$U$1&amp;")"</f>
-        <v>1624(22) (2015Su01)</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AA4" s="1">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" ht="12" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2519</v>
       </c>
@@ -732,18 +751,19 @@
         <v>22</v>
       </c>
       <c r="I5" s="9">
-        <f t="shared" ref="I5:I7" si="4">I16/36*35</f>
+        <f t="shared" ref="I5:I7" si="6">I16/36*35</f>
         <v>2548.1944444444443</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" si="1"/>
         <v>37.110372996651719</v>
       </c>
-      <c r="K5" s="10">
-        <f>K17*1/1.03-0.1</f>
-        <v>1.5504854368932037</v>
-      </c>
-      <c r="L5" s="4">
+      <c r="K5" s="5">
+        <f t="shared" si="2"/>
+        <v>37.799999999999997</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="M5" s="3">
@@ -754,20 +774,20 @@
         <f t="shared" si="0"/>
         <v>20.964862579157607</v>
       </c>
-      <c r="O5" s="4">
-        <f>O17</f>
-        <v>3.5</v>
-      </c>
-      <c r="P5" s="4">
-        <f>P17</f>
-        <v>5</v>
+      <c r="O5" s="1">
+        <f t="shared" ref="O5:P5" si="7">O16</f>
+        <v>37</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="Q5" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2537.5</v>
       </c>
       <c r="R5" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>17.5</v>
       </c>
       <c r="S5" s="1">
@@ -777,11 +797,11 @@
         <v>42</v>
       </c>
       <c r="U5" s="3">
-        <f t="shared" ref="U5:V5" si="5">U16/36*35</f>
+        <f t="shared" ref="U5:V5" si="8">U16/36*35</f>
         <v>2593.8888888888891</v>
       </c>
       <c r="V5" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>30.138888888888889</v>
       </c>
       <c r="W5" s="5">
@@ -790,46 +810,41 @@
       <c r="X5" s="1">
         <v>58</v>
       </c>
-      <c r="AB5" s="3" t="str">
-        <f>TEXT(A5, "0")&amp;"("&amp;TEXT(B5, "0")&amp;") ("&amp;$A$1&amp;"), "</f>
-        <v xml:space="preserve">2519(21) (1981Ay01), </v>
-      </c>
-      <c r="AC5" s="3" t="str">
-        <f>TEXT(E5, "0.0")&amp;"("&amp;TEXT(F5, "0")&amp;") ("&amp;$E$1&amp;"), "</f>
-        <v xml:space="preserve">2550.2(22) (1995Ga16), </v>
+      <c r="AA5" s="1">
+        <v>2549.9</v>
       </c>
       <c r="AD5" s="3" t="str">
-        <f>TEXT(I5, "0")&amp;"("&amp;TEXT(J5, "0")&amp;") ("&amp;$I$1&amp;"), "</f>
-        <v xml:space="preserve">2548(37) (1997Tr05), </v>
+        <f>TEXT(K4, "0.0")&amp;"("&amp;TEXT(L4, "0")&amp;") ("&amp;$I$1&amp;"), "</f>
+        <v xml:space="preserve">11.3(6) (1997Tr05), </v>
       </c>
       <c r="AE5" s="3" t="str">
-        <f>TEXT(M5, "0")&amp;"("&amp;TEXT(N5, "0")&amp;") ("&amp;$M$1&amp;"), "</f>
-        <v xml:space="preserve">2551(21) (2001Lo11), </v>
+        <f>TEXT(O4, "0.0")&amp;"("&amp;TEXT(P4, "0")&amp;") ("&amp;$M$1&amp;"), "</f>
+        <v xml:space="preserve">9.3(8) (2001Lo11), </v>
       </c>
       <c r="AF5" s="3" t="str">
-        <f>TEXT(Q5, "0")&amp;"("&amp;TEXT(R5, "0")&amp;") ("&amp;$Q$1&amp;"), "</f>
-        <v xml:space="preserve">2538(18) (2007Do17), </v>
+        <f>TEXT(S4, "0.0")&amp;"("&amp;TEXT(T4, "0")&amp;") ("&amp;$Q$1&amp;"), "</f>
+        <v xml:space="preserve">7.3(8) (2007Do17), </v>
       </c>
       <c r="AG5" s="3" t="str">
-        <f>TEXT(U5, "0")&amp;"("&amp;TEXT(V5, "0")&amp;") ("&amp;$U$1&amp;")"</f>
-        <v>2594(30) (2015Su01)</v>
+        <f>TEXT(W4, "0.0")&amp;"("&amp;TEXT(X4, "0")&amp;") ("&amp;$U$1&amp;")"</f>
+        <v>5.7(16) (2015Su01)</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="I6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2713.4722222222222</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" si="1"/>
         <v>31.126298376409682</v>
       </c>
-      <c r="K6" s="1">
-        <f>K18</f>
-        <v>1.4</v>
+      <c r="K6" s="5">
+        <f t="shared" si="2"/>
+        <v>1.7</v>
       </c>
       <c r="L6" s="1">
-        <f>L18</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M6" s="3">
@@ -841,38 +856,51 @@
         <v>20.964862579157607</v>
       </c>
       <c r="O6" s="1">
-        <f>O18</f>
-        <v>1</v>
+        <f t="shared" ref="O6:P6" si="9">O17</f>
+        <v>3.5</v>
       </c>
       <c r="P6" s="1">
-        <f>P18</f>
-        <v>3</v>
-      </c>
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>2713</v>
+      </c>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
       <c r="AD6" s="3" t="str">
-        <f t="shared" ref="AD6:AD11" si="6">TEXT(I6, "0")&amp;"("&amp;TEXT(J6, "0")&amp;") ("&amp;$I$1&amp;"), "</f>
-        <v xml:space="preserve">2713(31) (1997Tr05), </v>
+        <f>TEXT(K5, "0.0")&amp;"("&amp;TEXT(L5, "0")&amp;") ("&amp;$I$1&amp;"), "</f>
+        <v xml:space="preserve">37.8(10) (1997Tr05), </v>
       </c>
       <c r="AE6" s="3" t="str">
-        <f t="shared" ref="AE6:AE11" si="7">TEXT(M6, "0")&amp;"("&amp;TEXT(N6, "0")&amp;") ("&amp;$M$1&amp;"), "</f>
-        <v xml:space="preserve">2713(21) (2001Lo11), </v>
+        <f>TEXT(O5, "0")&amp;"("&amp;TEXT(P5, "0")&amp;") ("&amp;$M$1&amp;"), "</f>
+        <v xml:space="preserve">37(1) (2001Lo11), </v>
+      </c>
+      <c r="AF6" s="3" t="str">
+        <f>TEXT(S5, "0.0")&amp;"("&amp;TEXT(T5, "0")&amp;") ("&amp;$Q$1&amp;"), "</f>
+        <v xml:space="preserve">32.1(42) (2007Do17), </v>
+      </c>
+      <c r="AG6" s="3" t="str">
+        <f>TEXT(W5, "0.0")&amp;"("&amp;TEXT(X5, "0")&amp;") ("&amp;$U$1&amp;")"</f>
+        <v>34.0(58) (2015Su01)</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="I7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2937.0833333333335</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="1"/>
         <v>35.121317521477522</v>
       </c>
-      <c r="K7" s="1">
-        <f>K19</f>
-        <v>0</v>
+      <c r="K7" s="5">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
       </c>
       <c r="L7" s="1">
-        <f>L19</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="M7" s="3">
         <f t="shared" si="0"/>
@@ -883,26 +911,30 @@
         <v>44.040700872412707</v>
       </c>
       <c r="O7" s="5">
-        <f>O19</f>
-        <v>0.6</v>
+        <f t="shared" ref="O7:P7" si="10">O18</f>
+        <v>1</v>
       </c>
       <c r="P7" s="1">
-        <f>P19</f>
-        <v>2</v>
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>2921</v>
       </c>
       <c r="AD7" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">2937(35) (1997Tr05), </v>
+        <f>TEXT(K6, "0.0")&amp;"("&amp;TEXT(L6, "0")&amp;") ("&amp;$I$1&amp;"), "</f>
+        <v xml:space="preserve">1.7(2) (1997Tr05), </v>
       </c>
       <c r="AE7" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">2895(44) (2001Lo11), </v>
+        <f>TEXT(O6, "0.0")&amp;"("&amp;TEXT(P6, "0")&amp;") ("&amp;$M$1&amp;"), "</f>
+        <v xml:space="preserve">3.5(5) (2001Lo11), </v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="I8" s="3"/>
+      <c r="K8" s="5"/>
       <c r="M8" s="3">
-        <f t="shared" si="0"/>
+        <f>M19/36*35</f>
         <v>3484.4444444444443</v>
       </c>
       <c r="N8" s="3">
@@ -910,21 +942,28 @@
         <v>20.964862579157607</v>
       </c>
       <c r="O8" s="1">
-        <f>O20</f>
-        <v>0.9</v>
+        <f t="shared" ref="O8:P8" si="11">O19</f>
+        <v>0.6</v>
       </c>
       <c r="P8" s="1">
-        <f>P20</f>
-        <v>2</v>
-      </c>
-      <c r="AD8" s="3"/>
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>3484</v>
+      </c>
+      <c r="AD8" s="3" t="str">
+        <f>TEXT(K7, "0.0")&amp;"("&amp;TEXT(L7, "0")&amp;") ("&amp;$I$1&amp;"), "</f>
+        <v xml:space="preserve">1.4(2) (1997Tr05), </v>
+      </c>
       <c r="AE8" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">3484(21) (2001Lo11), </v>
+        <f t="shared" ref="AE8:AE12" si="12">TEXT(O7, "0.0")&amp;"("&amp;TEXT(P7, "0")&amp;") ("&amp;$M$1&amp;"), "</f>
+        <v xml:space="preserve">1.0(3) (2001Lo11), </v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="I9" s="3"/>
+      <c r="K9" s="5"/>
       <c r="M9" s="3">
         <f t="shared" si="0"/>
         <v>3981.25</v>
@@ -934,17 +973,20 @@
         <v>66.630922130423926</v>
       </c>
       <c r="O9" s="1">
-        <f>O21</f>
-        <v>1.7</v>
+        <f t="shared" ref="O9:P9" si="13">O20</f>
+        <v>0.9</v>
       </c>
       <c r="P9" s="1">
-        <f>P21</f>
-        <v>3</v>
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="AA9" s="13">
+        <v>3980</v>
       </c>
       <c r="AD9" s="3"/>
       <c r="AE9" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">3981(67) (2001Lo11), </v>
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">0.6(2) (2001Lo11), </v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
@@ -956,13 +998,13 @@
         <f>J21/36*35</f>
         <v>45.027640687981048</v>
       </c>
-      <c r="K10" s="1">
-        <f>K22</f>
-        <v>0.7</v>
+      <c r="K10" s="5">
+        <f t="shared" si="2"/>
+        <v>2.7</v>
       </c>
       <c r="L10" s="1">
-        <f>L22</f>
-        <v>2</v>
+        <f t="shared" ref="L8:L11" si="14">L21</f>
+        <v>4</v>
       </c>
       <c r="M10" s="3">
         <f t="shared" si="0"/>
@@ -973,20 +1015,20 @@
         <v>44.040700872412707</v>
       </c>
       <c r="O10" s="1">
-        <f>O22</f>
-        <v>0.3</v>
+        <f t="shared" ref="O10:P10" si="15">O21</f>
+        <v>1.7</v>
       </c>
       <c r="P10" s="1">
-        <f>P22</f>
-        <v>1</v>
-      </c>
-      <c r="AD10" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">4162(45) (1997Tr05), </v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="AA10" s="13">
+        <v>4150</v>
+      </c>
+      <c r="AD10" s="3"/>
       <c r="AE10" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">4135(44) (2001Lo11), </v>
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">0.9(2) (2001Lo11), </v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
@@ -998,13 +1040,13 @@
         <f>J22/36*35</f>
         <v>68.588193428444939</v>
       </c>
-      <c r="K11" s="1">
-        <f>K23</f>
-        <v>0</v>
+      <c r="K11" s="5">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
       </c>
       <c r="L11" s="1">
-        <f>L23</f>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>2</v>
       </c>
       <c r="M11" s="3">
         <f>M22/36*35</f>
@@ -1015,20 +1057,33 @@
         <v>66.630922130423926</v>
       </c>
       <c r="O11" s="1">
-        <f>O23</f>
-        <v>0</v>
+        <f t="shared" ref="O11:P11" si="16">O22</f>
+        <v>0.3</v>
       </c>
       <c r="P11" s="1">
-        <f>P23</f>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="AA11" s="13">
+        <v>4990</v>
       </c>
       <c r="AD11" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">4989(69) (1997Tr05), </v>
+        <f>TEXT(K10, "0.0")&amp;"("&amp;TEXT(L10, "0")&amp;") ("&amp;$I$1&amp;"), "</f>
+        <v xml:space="preserve">2.7(4) (1997Tr05), </v>
       </c>
       <c r="AE11" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">4983(67) (2001Lo11), </v>
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">1.7(3) (2001Lo11), </v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AD12" s="3" t="str">
+        <f>TEXT(K11, "0.0")&amp;"("&amp;TEXT(L11, "0")&amp;") ("&amp;$I$1&amp;"), "</f>
+        <v xml:space="preserve">0.7(2) (1997Tr05), </v>
+      </c>
+      <c r="AE12" s="3" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">0.3(1) (2001Lo11), </v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
@@ -1050,19 +1105,24 @@
       <c r="U13" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="I14" s="9">
+      <c r="AA13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" ht="12" x14ac:dyDescent="0.3">
+      <c r="I14" s="3">
         <f>I28-$I$25-1184</f>
         <v>1437</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="5">
-        <f>K28*0.03/1.03+0.1</f>
-        <v>1.2359223300970874</v>
+        <v>1.2</v>
       </c>
       <c r="L14" s="4"/>
-      <c r="M14" s="9">
+      <c r="M14" s="3">
         <f>M28-$M$25-1184</f>
         <v>1440</v>
       </c>
@@ -1097,11 +1157,11 @@
         <v>21.563858652847824</v>
       </c>
       <c r="O15" s="1">
-        <f>O27</f>
+        <f t="shared" ref="O15:P22" si="17">O27</f>
         <v>9.3000000000000007</v>
       </c>
       <c r="P15" s="1">
-        <f>P27</f>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="Q15" s="6">
@@ -1134,9 +1194,12 @@
       <c r="Z15" s="2">
         <v>0.8</v>
       </c>
-      <c r="AA15" s="2"/>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AA15" s="3">
+        <f>AA4/35*36</f>
+        <v>1695.0857142857144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" ht="12" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <f>A5/35*36</f>
         <v>2590.9714285714285</v>
@@ -1160,18 +1223,17 @@
         <v>38.17066936798463</v>
       </c>
       <c r="K16" s="10">
-        <f>K28*1/1.03-0.1</f>
-        <v>37.76407766990291</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="L16" s="4">
         <v>10</v>
       </c>
       <c r="M16" s="9">
-        <f t="shared" ref="M15:M21" si="8">M28-$M$25</f>
+        <f>M28-$M$25</f>
         <v>2624</v>
       </c>
       <c r="N16" s="4">
-        <f t="shared" ref="N15:N21" si="9">SQRT(N28^2-$N$25^2)</f>
+        <f t="shared" ref="N16:N21" si="18">SQRT(N28^2-$N$25^2)</f>
         <v>21.563858652847824</v>
       </c>
       <c r="O16" s="4">
@@ -1179,7 +1241,7 @@
         <v>37</v>
       </c>
       <c r="P16" s="4">
-        <f>P28</f>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="Q16" s="6">
@@ -1206,8 +1268,28 @@
       <c r="X16" s="6">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="AA16" s="5">
+        <f>AA5/35*36</f>
+        <v>2622.7542857142862</v>
+      </c>
+      <c r="AD16" s="3" t="str">
+        <f>TEXT(I4, "0")&amp;"("&amp;TEXT(J4, "0")&amp;") ("&amp;$I$1&amp;"), "</f>
+        <v xml:space="preserve">1676(39) (1997Tr05), </v>
+      </c>
+      <c r="AE16" s="3" t="str">
+        <f>TEXT(M4, "0")&amp;"("&amp;TEXT(N4, "0")&amp;") ("&amp;$M$1&amp;"), "</f>
+        <v xml:space="preserve">1645(21) (2001Lo11), </v>
+      </c>
+      <c r="AF16" s="3" t="str">
+        <f>TEXT(Q4, "0")&amp;"("&amp;TEXT(R4, "0")&amp;") ("&amp;$Q$1&amp;"), "</f>
+        <v xml:space="preserve">1660(18) (2007Do17), </v>
+      </c>
+      <c r="AG16" s="3" t="str">
+        <f>TEXT(U4, "0")&amp;"("&amp;TEXT(V4, "0")&amp;") ("&amp;$U$1&amp;")"</f>
+        <v>1624(22) (2015Su01)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="I17" s="3">
         <f>I29-$I$25</f>
         <v>2791</v>
@@ -1225,28 +1307,56 @@
         <v>2</v>
       </c>
       <c r="M17" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="M16:M21" si="19">M29-$M$25</f>
         <v>2791</v>
       </c>
       <c r="N17" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>21.563858652847824</v>
       </c>
       <c r="O17" s="1">
-        <f>O29</f>
+        <f t="shared" si="17"/>
         <v>3.5</v>
       </c>
       <c r="P17" s="1">
-        <f>P29</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="AA17" s="3">
+        <f t="shared" ref="AA16:AA22" si="20">AA6/35*36</f>
+        <v>2790.514285714286</v>
+      </c>
+      <c r="AB17" s="3" t="str">
+        <f>TEXT(A5, "0")&amp;"("&amp;TEXT(B5, "0")&amp;") ("&amp;$A$1&amp;"), "</f>
+        <v xml:space="preserve">2519(21) (1981Ay01), </v>
+      </c>
+      <c r="AC17" s="3" t="str">
+        <f>TEXT(E5, "0.0")&amp;"("&amp;TEXT(F5, "0")&amp;") ("&amp;$E$1&amp;"), "</f>
+        <v xml:space="preserve">2550.2(22) (1995Ga16), </v>
+      </c>
+      <c r="AD17" s="3" t="str">
+        <f>TEXT(I5, "0")&amp;"("&amp;TEXT(J5, "0")&amp;") ("&amp;$I$1&amp;"), "</f>
+        <v xml:space="preserve">2548(37) (1997Tr05), </v>
+      </c>
+      <c r="AE17" s="3" t="str">
+        <f>TEXT(M5, "0")&amp;"("&amp;TEXT(N5, "0")&amp;") ("&amp;$M$1&amp;"), "</f>
+        <v xml:space="preserve">2551(21) (2001Lo11), </v>
+      </c>
+      <c r="AF17" s="3" t="str">
+        <f>TEXT(Q5, "0")&amp;"("&amp;TEXT(R5, "0")&amp;") ("&amp;$Q$1&amp;"), "</f>
+        <v xml:space="preserve">2538(18) (2007Do17), </v>
+      </c>
+      <c r="AG17" s="3" t="str">
+        <f>TEXT(U5, "0")&amp;"("&amp;TEXT(V5, "0")&amp;") ("&amp;$U$1&amp;")"</f>
+        <v>2594(30) (2015Su01)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="I18" s="3">
         <f>I30-$I$25</f>
         <v>3021</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="3">
         <f>SQRT(J30^2-$J$25^2)</f>
         <v>36.124783736376884</v>
       </c>
@@ -1259,61 +1369,94 @@
         <v>2</v>
       </c>
       <c r="M18" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>2978</v>
       </c>
       <c r="N18" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>45.299006611624499</v>
       </c>
       <c r="O18" s="5">
-        <f>O30</f>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="P18" s="1">
-        <f>P30</f>
+        <f t="shared" si="17"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="AA18" s="3">
+        <f t="shared" si="20"/>
+        <v>3004.4571428571426</v>
+      </c>
+      <c r="AD18" s="3" t="str">
+        <f>TEXT(I6, "0")&amp;"("&amp;TEXT(J6, "0")&amp;") ("&amp;$I$1&amp;"), "</f>
+        <v xml:space="preserve">2713(31) (1997Tr05), </v>
+      </c>
+      <c r="AE18" s="3" t="str">
+        <f>TEXT(M6, "0")&amp;"("&amp;TEXT(N6, "0")&amp;") ("&amp;$M$1&amp;"), "</f>
+        <v xml:space="preserve">2713(21) (2001Lo11), </v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="I19" s="3"/>
       <c r="M19" s="3">
-        <f t="shared" si="8"/>
+        <f>M31-$M$25</f>
         <v>3584</v>
       </c>
       <c r="N19" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>21.563858652847824</v>
       </c>
       <c r="O19" s="1">
-        <f>O31</f>
+        <f t="shared" si="17"/>
         <v>0.6</v>
       </c>
       <c r="P19" s="1">
-        <f>P31</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="AA19" s="3">
+        <f t="shared" si="20"/>
+        <v>3583.5428571428574</v>
+      </c>
+      <c r="AD19" s="3" t="str">
+        <f>TEXT(I7, "0")&amp;"("&amp;TEXT(J7, "0")&amp;") ("&amp;$I$1&amp;"), "</f>
+        <v xml:space="preserve">2937(35) (1997Tr05), </v>
+      </c>
+      <c r="AE19" s="3" t="str">
+        <f>TEXT(M7, "0")&amp;"("&amp;TEXT(N7, "0")&amp;") ("&amp;$M$1&amp;"), "</f>
+        <v xml:space="preserve">2895(44) (2001Lo11), </v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="I20" s="3"/>
       <c r="M20" s="3">
-        <f t="shared" si="8"/>
+        <f>M32-$M$25</f>
         <v>4095</v>
       </c>
       <c r="N20" s="1">
-        <f t="shared" si="9"/>
+        <f>SQRT(N32^2-$N$25^2)</f>
         <v>68.534662762721752</v>
       </c>
       <c r="O20" s="1">
-        <f>O32</f>
+        <f t="shared" si="17"/>
         <v>0.9</v>
       </c>
       <c r="P20" s="1">
-        <f>P32</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="AA20" s="3">
+        <f t="shared" si="20"/>
+        <v>4093.7142857142853</v>
+      </c>
+      <c r="AD20" s="3"/>
+      <c r="AE20" s="3" t="str">
+        <f>TEXT(M8, "0")&amp;"("&amp;TEXT(N8, "0")&amp;") ("&amp;$M$1&amp;"), "</f>
+        <v xml:space="preserve">3484(21) (2001Lo11), </v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="I21" s="3">
         <f>I33-$I$25</f>
         <v>4281</v>
@@ -1331,23 +1474,32 @@
         <v>4</v>
       </c>
       <c r="M21" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>4253</v>
       </c>
       <c r="N21" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>45.299006611624499</v>
       </c>
       <c r="O21" s="1">
-        <f>O33</f>
+        <f t="shared" si="17"/>
         <v>1.7</v>
       </c>
       <c r="P21" s="1">
-        <f>P33</f>
+        <f t="shared" si="17"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="AA21" s="3">
+        <f t="shared" si="20"/>
+        <v>4268.5714285714284</v>
+      </c>
+      <c r="AD21" s="3"/>
+      <c r="AE21" s="3" t="str">
+        <f>TEXT(M9, "0")&amp;"("&amp;TEXT(N9, "0")&amp;") ("&amp;$M$1&amp;"), "</f>
+        <v xml:space="preserve">3981(67) (2001Lo11), </v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="I22" s="3">
         <f>I34-$I$25</f>
         <v>5132</v>
@@ -1373,18 +1525,39 @@
         <v>68.534662762721752</v>
       </c>
       <c r="O22" s="1">
-        <f>O34</f>
+        <f t="shared" si="17"/>
         <v>0.3</v>
       </c>
       <c r="P22" s="1">
-        <f>P34</f>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="AA22" s="3">
+        <f t="shared" si="20"/>
+        <v>5132.5714285714294</v>
+      </c>
+      <c r="AD22" s="3" t="str">
+        <f>TEXT(I10, "0")&amp;"("&amp;TEXT(J10, "0")&amp;") ("&amp;$I$1&amp;"), "</f>
+        <v xml:space="preserve">4162(45) (1997Tr05), </v>
+      </c>
+      <c r="AE22" s="3" t="str">
+        <f>TEXT(M10, "0")&amp;"("&amp;TEXT(N10, "0")&amp;") ("&amp;$M$1&amp;"), "</f>
+        <v xml:space="preserve">4135(44) (2001Lo11), </v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="K23" s="5"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="AA23" s="3"/>
+      <c r="AD23" s="3" t="str">
+        <f>TEXT(I11, "0")&amp;"("&amp;TEXT(J11, "0")&amp;") ("&amp;$I$1&amp;"), "</f>
+        <v xml:space="preserve">4989(69) (1997Tr05), </v>
+      </c>
+      <c r="AE23" s="3" t="str">
+        <f>TEXT(M11, "0")&amp;"("&amp;TEXT(N11, "0")&amp;") ("&amp;$M$1&amp;"), "</f>
+        <v xml:space="preserve">4983(67) (2001Lo11), </v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="I24" s="2" t="s">
         <v>1</v>
       </c>
@@ -1393,8 +1566,9 @@
         <v>1</v>
       </c>
       <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="AA24" s="3"/>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="I25" s="2">
         <v>1666</v>
       </c>
@@ -1407,8 +1581,9 @@
       <c r="N25" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="AA25" s="3"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1427,8 +1602,11 @@
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="8"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="AA26" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f>M16+$Y$15</f>
         <v>4282.8999999999996</v>
@@ -1461,8 +1639,12 @@
       <c r="P27" s="6">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="AA27" s="3">
+        <f>AA15+$Y$4</f>
+        <v>3353.9857142857145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" ht="12" x14ac:dyDescent="0.3">
       <c r="I28" s="11">
         <v>4287</v>
       </c>
@@ -1487,8 +1669,12 @@
       <c r="P28" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="AA28" s="5">
+        <f>AA16+$Y$4</f>
+        <v>4281.6542857142867</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="I29" s="6">
         <v>4457</v>
       </c>
@@ -1513,8 +1699,12 @@
       <c r="P29" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="AA29" s="3">
+        <f>AA17+$Y$4</f>
+        <v>4449.4142857142861</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="I30" s="6">
         <v>4687</v>
       </c>
@@ -1539,8 +1729,12 @@
       <c r="P30" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="AA30" s="3">
+        <f>AA18+$Y$4</f>
+        <v>4663.3571428571431</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
@@ -1557,8 +1751,12 @@
       <c r="P31" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="AA31" s="3">
+        <f>AA19+$Y$4</f>
+        <v>5242.442857142858</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
@@ -1575,8 +1773,12 @@
       <c r="P32" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="AA32" s="3">
+        <f>AA20+$Y$4</f>
+        <v>5752.6142857142859</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="I33" s="6">
         <v>5947</v>
       </c>
@@ -1601,8 +1803,12 @@
       <c r="P33" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="AA33" s="3">
+        <f>AA21+$Y$4</f>
+        <v>5927.471428571429</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="I34" s="6">
         <v>6798</v>
       </c>
@@ -1626,6 +1832,20 @@
       </c>
       <c r="P34" s="6">
         <v>1</v>
+      </c>
+      <c r="AA34" s="3">
+        <f>AA22+$Y$4</f>
+        <v>6791.471428571429</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A35" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A36" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>